<commit_message>
added images for plots and edited scratchpad and index.html
</commit_message>
<xml_diff>
--- a/movies_data_scratchpad.xlsx
+++ b/movies_data_scratchpad.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sixonecom-my.sharepoint.com/personal/scottkutlick_61commodities_com/Documents/Documents/GitHub/project-03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{F24E202F-3D40-41AA-889A-C3C095DB346A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DF4A4B7-AFE9-4FA4-A6BF-BCA2865157CC}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{F24E202F-3D40-41AA-889A-C3C095DB346A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C0F42DC-FF12-47A4-9B14-0FBACE3AE36D}"/>
   <bookViews>
-    <workbookView xWindow="39070" yWindow="130" windowWidth="28800" windowHeight="21150" activeTab="1" xr2:uid="{F217124C-1929-4560-B9AF-CC2EABF9FC7B}"/>
+    <workbookView xWindow="57600" yWindow="0" windowWidth="19200" windowHeight="21600" activeTab="1" xr2:uid="{F217124C-1929-4560-B9AF-CC2EABF9FC7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$Q$501</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$Q$501</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$A$1:$G$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2197" uniqueCount="1040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2202" uniqueCount="1045">
   <si>
     <t>rank</t>
   </si>
@@ -3185,6 +3187,21 @@
   </si>
   <si>
     <t>1991','1994','1995','1996','1997','1998','1999','2000','2001','2002','2003','2004','2005','2006','2007','2008','2009','2010','2011','2012','2013','2014','2015','2016','2017','2018','2019','2020','2021','2022','2023','NA'</t>
+  </si>
+  <si>
+    <t>Top 500 Movies (by Production Cost)</t>
+  </si>
+  <si>
+    <t>Production Cost vs. Worldwide Gross</t>
+  </si>
+  <si>
+    <t>Ratings Distribution</t>
+  </si>
+  <si>
+    <t>Movie Releases</t>
+  </si>
+  <si>
+    <t>Opening Weekend</t>
   </si>
 </sst>
 </file>
@@ -3211,7 +3228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3230,8 +3247,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -3239,11 +3274,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3258,6 +3319,23 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8442,6 +8520,62 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="138"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -10408,6 +10542,316 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>600809</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177863</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CF8AAF0-81A7-C9EE-2FAB-0E8EA2B0053E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1" y="591040"/>
+          <a:ext cx="2779346" cy="2204977"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>483577</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>63506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>706165</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F8C720B-95CC-E3CE-E7C2-B01DC6FC17B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3883269" y="635006"/>
+          <a:ext cx="2743050" cy="2188308"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>410308</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>166079</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>312616</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>115778</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C16D453-5C5D-1CE2-F574-89A2F167B51B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="410308" y="3355733"/>
+          <a:ext cx="2080846" cy="2181968"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>322385</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>43962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>932962</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>81037</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6738BF9F-BE7E-0129-4681-F7A15143371C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3111500" y="3424116"/>
+          <a:ext cx="3741616" cy="2078844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>97692</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>83040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1068365</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>34193</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E3B754D-8629-0DF8-4E1E-D702A46CE3AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="97692" y="6061809"/>
+          <a:ext cx="6890827" cy="1250461"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -20037,7 +20481,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{230D1068-DE9B-439F-8469-BC3F9A2F28BB}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{230D1068-DE9B-439F-8469-BC3F9A2F28BB}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A3:H37" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="17">
     <pivotField showAll="0"/>
@@ -20255,7 +20699,7 @@
   <dataFields count="1">
     <dataField name="Sum of worldwide_net" fld="14" baseField="12" baseItem="0" numFmtId="38"/>
   </dataFields>
-  <chartFormats count="160">
+  <chartFormats count="167">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -22440,6 +22884,90 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="0" format="138" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="145" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="146" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="147" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="148" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="149" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="150" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -23616,14 +24144,571 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734592B2-0715-4500-84B7-376874C7D5BA}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.90625" customWidth="1"/>
+    <col min="7" max="7" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="17" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="19" t="s">
+        <v>1043</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="16"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="17" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="19" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E17:F17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="87" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F0A281-E009-4D86-9ABF-34151765EA45}">
   <dimension ref="A1:V604"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D460" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J504" sqref="J504"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>